<commit_message>
Two of many done
</commit_message>
<xml_diff>
--- a/final_stuff/FinalProject_Primary_Review1.xlsx
+++ b/final_stuff/FinalProject_Primary_Review1.xlsx
@@ -442,8 +442,8 @@
   </sheetPr>
   <dimension ref="A1:F39"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C39" activeCellId="0" sqref="C39"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>